<commit_message>
fix + validate user
</commit_message>
<xml_diff>
--- a/packages/backend/ScheduleReport.xlsx
+++ b/packages/backend/ScheduleReport.xlsx
@@ -397,10 +397,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" customWidth="1" width="16"/>
+    <col min="2" max="2" customWidth="1" width="24"/>
+    <col min="3" max="3" customWidth="1" width="16"/>
+    <col min="4" max="4" customWidth="1" width="44"/>
+    <col min="5" max="5" customWidth="1" width="16"/>
+    <col min="6" max="6" customWidth="1" width="24"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -424,16 +432,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>19110373</v>
+        <v>19110373,19110327</v>
       </c>
       <c r="B2" t="str">
-        <v>Pham Quang Hung</v>
+        <v>Pham Quang Hung,Le Quoc Bao</v>
       </c>
       <c r="C2" t="str">
-        <v>TLCN-2</v>
+        <v>22-TLCN-1</v>
       </c>
       <c r="D2" t="str">
-        <v>ssssssssss</v>
+        <v>Xây dụng web thương mại điện tử e-shop</v>
       </c>
       <c r="E2" t="str">
         <v>2000</v>
@@ -444,27 +452,287 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>19110323</v>
+        <v/>
       </c>
       <c r="B3" t="str">
-        <v>Ta Quoc Anh</v>
+        <v/>
       </c>
       <c r="C3" t="str">
-        <v>TLCN CNTT-3</v>
+        <v>TL-13</v>
       </c>
       <c r="D3" t="str">
-        <v>hung</v>
+        <v>HUDHJDHJ</v>
       </c>
       <c r="E3" t="str">
         <v>2000</v>
       </c>
       <c r="F3" t="str">
+        <v>LECTURER HUNG</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v/>
+      </c>
+      <c r="B4" t="str">
+        <v/>
+      </c>
+      <c r="C4" t="str">
+        <v>TL-10</v>
+      </c>
+      <c r="D4" t="str">
+        <v>HUDHJDHJ</v>
+      </c>
+      <c r="E4" t="str">
+        <v>2000</v>
+      </c>
+      <c r="F4" t="str">
+        <v>LECTURER HUNG</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v/>
+      </c>
+      <c r="B5" t="str">
+        <v/>
+      </c>
+      <c r="C5" t="str">
+        <v>TL-7</v>
+      </c>
+      <c r="D5" t="str">
+        <v>HUDHJDHJ</v>
+      </c>
+      <c r="E5" t="str">
+        <v>2000</v>
+      </c>
+      <c r="F5" t="str">
+        <v>LECTURER HUNG</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v/>
+      </c>
+      <c r="B6" t="str">
+        <v/>
+      </c>
+      <c r="C6" t="str">
+        <v>TL-9</v>
+      </c>
+      <c r="D6" t="str">
+        <v>HUDHJDHJ</v>
+      </c>
+      <c r="E6" t="str">
+        <v>2000</v>
+      </c>
+      <c r="F6" t="str">
+        <v>LECTURER HUNG</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v/>
+      </c>
+      <c r="B7" t="str">
+        <v/>
+      </c>
+      <c r="C7" t="str">
+        <v>TL-4</v>
+      </c>
+      <c r="D7" t="str">
+        <v>HUDHJDHJ</v>
+      </c>
+      <c r="E7" t="str">
+        <v>2000</v>
+      </c>
+      <c r="F7" t="str">
+        <v>LECTURER HUNG</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v/>
+      </c>
+      <c r="B8" t="str">
+        <v/>
+      </c>
+      <c r="C8" t="str">
+        <v>TL-8</v>
+      </c>
+      <c r="D8" t="str">
+        <v>HUDHJDHJ</v>
+      </c>
+      <c r="E8" t="str">
+        <v>2000</v>
+      </c>
+      <c r="F8" t="str">
+        <v>LECTURER HUNG</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v/>
+      </c>
+      <c r="B9" t="str">
+        <v/>
+      </c>
+      <c r="C9" t="str">
+        <v>TL-5</v>
+      </c>
+      <c r="D9" t="str">
+        <v>HUDHJDHJ</v>
+      </c>
+      <c r="E9" t="str">
+        <v>2000</v>
+      </c>
+      <c r="F9" t="str">
+        <v>LECTURER HUNG</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v/>
+      </c>
+      <c r="B10" t="str">
+        <v/>
+      </c>
+      <c r="C10" t="str">
+        <v>TL-2</v>
+      </c>
+      <c r="D10" t="str">
+        <v>HUDHJDHJ</v>
+      </c>
+      <c r="E10" t="str">
+        <v>2000</v>
+      </c>
+      <c r="F10" t="str">
+        <v>LECTURER HUNG</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v/>
+      </c>
+      <c r="B11" t="str">
+        <v/>
+      </c>
+      <c r="C11" t="str">
+        <v>TL-3</v>
+      </c>
+      <c r="D11" t="str">
+        <v>HUDHJDHJ</v>
+      </c>
+      <c r="E11" t="str">
+        <v>2000</v>
+      </c>
+      <c r="F11" t="str">
+        <v>LECTURER HUNG</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v/>
+      </c>
+      <c r="B12" t="str">
+        <v/>
+      </c>
+      <c r="C12" t="str">
+        <v>TL-1</v>
+      </c>
+      <c r="D12" t="str">
+        <v>HUDHJDHJ</v>
+      </c>
+      <c r="E12" t="str">
+        <v>2000</v>
+      </c>
+      <c r="F12" t="str">
+        <v>LECTURER HUNG</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v/>
+      </c>
+      <c r="B13" t="str">
+        <v/>
+      </c>
+      <c r="C13" t="str">
+        <v>TL-12</v>
+      </c>
+      <c r="D13" t="str">
+        <v>HUDHJDHJ</v>
+      </c>
+      <c r="E13" t="str">
+        <v>2000</v>
+      </c>
+      <c r="F13" t="str">
+        <v>LECTURER HUNG</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v/>
+      </c>
+      <c r="B14" t="str">
+        <v/>
+      </c>
+      <c r="C14" t="str">
+        <v>TL-6</v>
+      </c>
+      <c r="D14" t="str">
+        <v>HUDHJDHJ</v>
+      </c>
+      <c r="E14" t="str">
+        <v>2000</v>
+      </c>
+      <c r="F14" t="str">
+        <v>LECTURER HUNG</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v/>
+      </c>
+      <c r="B15" t="str">
+        <v/>
+      </c>
+      <c r="C15" t="str">
+        <v>TL-14</v>
+      </c>
+      <c r="D15" t="str">
+        <v>HUDHJDHJ</v>
+      </c>
+      <c r="E15" t="str">
+        <v>2000</v>
+      </c>
+      <c r="F15" t="str">
+        <v>LECTURER HUNG</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v/>
+      </c>
+      <c r="B16" t="str">
+        <v/>
+      </c>
+      <c r="C16" t="str">
+        <v>TL-11</v>
+      </c>
+      <c r="D16" t="str">
+        <v>HUDHJDHJ</v>
+      </c>
+      <c r="E16" t="str">
+        <v>2000</v>
+      </c>
+      <c r="F16" t="str">
         <v>LECTURER HUNG</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F16"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix UI + export
</commit_message>
<xml_diff>
--- a/packages/backend/ScheduleReport.xlsx
+++ b/packages/backend/ScheduleReport.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -408,6 +408,8 @@
     <col min="4" max="4" customWidth="1" width="44"/>
     <col min="5" max="5" customWidth="1" width="16"/>
     <col min="6" max="6" customWidth="1" width="24"/>
+    <col min="7" max="7" customWidth="1" width="16"/>
+    <col min="8" max="8" customWidth="1" width="24"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -429,24 +431,36 @@
       <c r="F1" t="str">
         <v>LECTURER NAME</v>
       </c>
+      <c r="G1" t="str">
+        <v>CRITICAL CODE</v>
+      </c>
+      <c r="H1" t="str">
+        <v>CRITICAL NAME</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>19110373,19110327</v>
+        <v>19110373</v>
       </c>
       <c r="B2" t="str">
-        <v>Pham Quang Hung,Le Quoc Bao</v>
+        <v>Pham Quang Hung</v>
       </c>
       <c r="C2" t="str">
-        <v>22-TLCN-1</v>
+        <v>TL-10</v>
       </c>
       <c r="D2" t="str">
-        <v>Xây dụng web thương mại điện tử e-shop</v>
+        <v>HUDHJDHJ</v>
       </c>
       <c r="E2" t="str">
         <v>2000</v>
       </c>
       <c r="F2" t="str">
+        <v>LECTURER HUNG</v>
+      </c>
+      <c r="G2" t="str">
+        <v>2000</v>
+      </c>
+      <c r="H2" t="str">
         <v>LECTURER HUNG</v>
       </c>
     </row>
@@ -458,7 +472,7 @@
         <v/>
       </c>
       <c r="C3" t="str">
-        <v>TL-13</v>
+        <v>TL-9</v>
       </c>
       <c r="D3" t="str">
         <v>HUDHJDHJ</v>
@@ -467,6 +481,12 @@
         <v>2000</v>
       </c>
       <c r="F3" t="str">
+        <v>LECTURER HUNG</v>
+      </c>
+      <c r="G3" t="str">
+        <v>2000</v>
+      </c>
+      <c r="H3" t="str">
         <v>LECTURER HUNG</v>
       </c>
     </row>
@@ -478,7 +498,7 @@
         <v/>
       </c>
       <c r="C4" t="str">
-        <v>TL-10</v>
+        <v>TL-4</v>
       </c>
       <c r="D4" t="str">
         <v>HUDHJDHJ</v>
@@ -487,6 +507,12 @@
         <v>2000</v>
       </c>
       <c r="F4" t="str">
+        <v>LECTURER HUNG</v>
+      </c>
+      <c r="G4" t="str">
+        <v>2000</v>
+      </c>
+      <c r="H4" t="str">
         <v>LECTURER HUNG</v>
       </c>
     </row>
@@ -498,7 +524,7 @@
         <v/>
       </c>
       <c r="C5" t="str">
-        <v>TL-7</v>
+        <v>TL-8</v>
       </c>
       <c r="D5" t="str">
         <v>HUDHJDHJ</v>
@@ -507,6 +533,12 @@
         <v>2000</v>
       </c>
       <c r="F5" t="str">
+        <v>LECTURER HUNG</v>
+      </c>
+      <c r="G5" t="str">
+        <v>2000</v>
+      </c>
+      <c r="H5" t="str">
         <v>LECTURER HUNG</v>
       </c>
     </row>
@@ -518,7 +550,7 @@
         <v/>
       </c>
       <c r="C6" t="str">
-        <v>TL-9</v>
+        <v>TL-5</v>
       </c>
       <c r="D6" t="str">
         <v>HUDHJDHJ</v>
@@ -527,6 +559,12 @@
         <v>2000</v>
       </c>
       <c r="F6" t="str">
+        <v>LECTURER HUNG</v>
+      </c>
+      <c r="G6" t="str">
+        <v>2000</v>
+      </c>
+      <c r="H6" t="str">
         <v>LECTURER HUNG</v>
       </c>
     </row>
@@ -538,7 +576,7 @@
         <v/>
       </c>
       <c r="C7" t="str">
-        <v>TL-4</v>
+        <v>TL-2</v>
       </c>
       <c r="D7" t="str">
         <v>HUDHJDHJ</v>
@@ -547,6 +585,12 @@
         <v>2000</v>
       </c>
       <c r="F7" t="str">
+        <v>LECTURER HUNG</v>
+      </c>
+      <c r="G7" t="str">
+        <v>2000</v>
+      </c>
+      <c r="H7" t="str">
         <v>LECTURER HUNG</v>
       </c>
     </row>
@@ -558,7 +602,7 @@
         <v/>
       </c>
       <c r="C8" t="str">
-        <v>TL-8</v>
+        <v>TL-3</v>
       </c>
       <c r="D8" t="str">
         <v>HUDHJDHJ</v>
@@ -567,6 +611,12 @@
         <v>2000</v>
       </c>
       <c r="F8" t="str">
+        <v>LECTURER HUNG</v>
+      </c>
+      <c r="G8" t="str">
+        <v>2000</v>
+      </c>
+      <c r="H8" t="str">
         <v>LECTURER HUNG</v>
       </c>
     </row>
@@ -578,7 +628,7 @@
         <v/>
       </c>
       <c r="C9" t="str">
-        <v>TL-5</v>
+        <v>TL-12</v>
       </c>
       <c r="D9" t="str">
         <v>HUDHJDHJ</v>
@@ -587,6 +637,12 @@
         <v>2000</v>
       </c>
       <c r="F9" t="str">
+        <v>LECTURER HUNG</v>
+      </c>
+      <c r="G9" t="str">
+        <v>2000</v>
+      </c>
+      <c r="H9" t="str">
         <v>LECTURER HUNG</v>
       </c>
     </row>
@@ -598,7 +654,7 @@
         <v/>
       </c>
       <c r="C10" t="str">
-        <v>TL-2</v>
+        <v>TL-6</v>
       </c>
       <c r="D10" t="str">
         <v>HUDHJDHJ</v>
@@ -607,6 +663,12 @@
         <v>2000</v>
       </c>
       <c r="F10" t="str">
+        <v>LECTURER HUNG</v>
+      </c>
+      <c r="G10" t="str">
+        <v>2000</v>
+      </c>
+      <c r="H10" t="str">
         <v>LECTURER HUNG</v>
       </c>
     </row>
@@ -618,7 +680,7 @@
         <v/>
       </c>
       <c r="C11" t="str">
-        <v>TL-3</v>
+        <v>TL-14</v>
       </c>
       <c r="D11" t="str">
         <v>HUDHJDHJ</v>
@@ -627,6 +689,12 @@
         <v>2000</v>
       </c>
       <c r="F11" t="str">
+        <v>LECTURER HUNG</v>
+      </c>
+      <c r="G11" t="str">
+        <v>2000</v>
+      </c>
+      <c r="H11" t="str">
         <v>LECTURER HUNG</v>
       </c>
     </row>
@@ -638,7 +706,7 @@
         <v/>
       </c>
       <c r="C12" t="str">
-        <v>TL-1</v>
+        <v>TL-11</v>
       </c>
       <c r="D12" t="str">
         <v>HUDHJDHJ</v>
@@ -649,90 +717,16 @@
       <c r="F12" t="str">
         <v>LECTURER HUNG</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v/>
-      </c>
-      <c r="B13" t="str">
-        <v/>
-      </c>
-      <c r="C13" t="str">
-        <v>TL-12</v>
-      </c>
-      <c r="D13" t="str">
-        <v>HUDHJDHJ</v>
-      </c>
-      <c r="E13" t="str">
-        <v>2000</v>
-      </c>
-      <c r="F13" t="str">
-        <v>LECTURER HUNG</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v/>
-      </c>
-      <c r="B14" t="str">
-        <v/>
-      </c>
-      <c r="C14" t="str">
-        <v>TL-6</v>
-      </c>
-      <c r="D14" t="str">
-        <v>HUDHJDHJ</v>
-      </c>
-      <c r="E14" t="str">
-        <v>2000</v>
-      </c>
-      <c r="F14" t="str">
-        <v>LECTURER HUNG</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v/>
-      </c>
-      <c r="B15" t="str">
-        <v/>
-      </c>
-      <c r="C15" t="str">
-        <v>TL-14</v>
-      </c>
-      <c r="D15" t="str">
-        <v>HUDHJDHJ</v>
-      </c>
-      <c r="E15" t="str">
-        <v>2000</v>
-      </c>
-      <c r="F15" t="str">
-        <v>LECTURER HUNG</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v/>
-      </c>
-      <c r="B16" t="str">
-        <v/>
-      </c>
-      <c r="C16" t="str">
-        <v>TL-11</v>
-      </c>
-      <c r="D16" t="str">
-        <v>HUDHJDHJ</v>
-      </c>
-      <c r="E16" t="str">
-        <v>2000</v>
-      </c>
-      <c r="F16" t="str">
+      <c r="G12" t="str">
+        <v>2000</v>
+      </c>
+      <c r="H12" t="str">
         <v>LECTURER HUNG</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F16"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>